<commit_message>
Updated simulator_cache.xlsx with ex3 from Lab3 pdf
</commit_message>
<xml_diff>
--- a/Raul_Tomusca/Lab3/simulator_cache.xlsx
+++ b/Raul_Tomusca/Lab3/simulator_cache.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\frost\OneDrive\Documents\Facultate\AN4\Soac\Lab1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/f07d9eb667e2e59f/Documents/Facultate/AN4/Soac/Lab3/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D386853-233C-4631-83ED-85E327878D2A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{1D386853-233C-4631-83ED-85E327878D2A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1084FFE0-F302-439A-8B56-65C853560203}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{42FF4CD8-4F1B-4B6C-9A88-8B7724198304}"/>
   </bookViews>
@@ -509,15 +509,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
@@ -543,6 +534,15 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="25" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="26" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="27" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -630,7 +630,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-CH"/>
+          <a:endParaRPr lang="LID4096"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -1459,7 +1459,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-CH"/>
+            <a:endParaRPr lang="LID4096"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1030845471"/>
@@ -1518,7 +1518,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-CH"/>
+            <a:endParaRPr lang="LID4096"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1030845055"/>
@@ -1560,7 +1560,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-CH"/>
+          <a:endParaRPr lang="LID4096"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -1590,7 +1590,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-CH"/>
+      <a:endParaRPr lang="LID4096"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -1666,7 +1666,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-CH"/>
+          <a:endParaRPr lang="LID4096"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -2495,7 +2495,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-CH"/>
+            <a:endParaRPr lang="LID4096"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1101207823"/>
@@ -2554,7 +2554,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-CH"/>
+            <a:endParaRPr lang="LID4096"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1101201167"/>
@@ -2596,7 +2596,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-CH"/>
+          <a:endParaRPr lang="LID4096"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -2626,7 +2626,2097 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-CH"/>
+      <a:endParaRPr lang="LID4096"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Issue</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> Rate</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.40949300087489071"/>
+          <c:y val="3.2407407407407406E-2"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="LID4096"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$C$50</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>64</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$B$51:$B$58</c:f>
+              <c:strCache>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>Sort</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Bubble</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Matrix</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Perm</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Puzzle</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Queens</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Tower</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Tree</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$C$51:$C$58</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>0.52900000000000003</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.55700000000000005</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.44500000000000001</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.43</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.41899999999999998</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.39100000000000001</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.443</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.35799999999999998</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-AE3A-4D9F-95A0-33FB5FBC7371}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$D$50</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>128</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$B$51:$B$58</c:f>
+              <c:strCache>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>Sort</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Bubble</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Matrix</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Perm</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Puzzle</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Queens</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Tower</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Tree</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$D$51:$D$58</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>0.56699999999999995</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.56799999999999995</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.502</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.42299999999999999</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.41899999999999998</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.497</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.373</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-AE3A-4D9F-95A0-33FB5FBC7371}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$E$50</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>256</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent3"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$B$51:$B$58</c:f>
+              <c:strCache>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>Sort</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Bubble</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Matrix</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Perm</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Puzzle</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Queens</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Tower</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Tree</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$E$51:$E$58</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>0.63800000000000001</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.62</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.55700000000000005</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.60699999999999998</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.443</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.48399999999999999</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.52400000000000002</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.40200000000000002</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-AE3A-4D9F-95A0-33FB5FBC7371}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$F$50</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>512</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent4"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$B$51:$B$58</c:f>
+              <c:strCache>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>Sort</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Bubble</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Matrix</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Perm</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Puzzle</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Queens</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Tower</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Tree</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$F$51:$F$58</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>0.70099999999999996</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.91600000000000004</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.624</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.66700000000000004</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.46899999999999997</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.63</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.67300000000000004</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.44600000000000001</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-AE3A-4D9F-95A0-33FB5FBC7371}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$G$50</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>1024</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent5"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$B$51:$B$58</c:f>
+              <c:strCache>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>Sort</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Bubble</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Matrix</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Perm</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Puzzle</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Queens</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Tower</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Tree</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$G$51:$G$58</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>0.77300000000000002</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.2190000000000001</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.65400000000000003</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.67</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.49199999999999999</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.69199999999999995</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.73199999999999998</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.51400000000000001</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000004-AE3A-4D9F-95A0-33FB5FBC7371}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$H$50</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>2048</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent6"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$B$51:$B$58</c:f>
+              <c:strCache>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>Sort</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Bubble</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Matrix</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Perm</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Puzzle</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Queens</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Tower</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Tree</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$H$51:$H$58</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>0.875</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.2190000000000001</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.85699999999999998</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.67</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.51400000000000001</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.82299999999999995</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.73599999999999999</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.58599999999999997</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000005-AE3A-4D9F-95A0-33FB5FBC7371}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="6"/>
+          <c:order val="6"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$I$50</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>4096</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1">
+                <a:lumMod val="60000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$B$51:$B$58</c:f>
+              <c:strCache>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>Sort</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Bubble</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Matrix</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Perm</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Puzzle</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Queens</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Tower</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Tree</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$I$51:$I$58</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>0.88900000000000001</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.2190000000000001</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.1759999999999999</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.67</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.55800000000000005</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.82299999999999995</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.89800000000000002</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.625</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000006-AE3A-4D9F-95A0-33FB5FBC7371}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="7"/>
+          <c:order val="7"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$J$50</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>8192</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2">
+                <a:lumMod val="60000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$B$51:$B$58</c:f>
+              <c:strCache>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>Sort</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Bubble</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Matrix</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Perm</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Puzzle</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Queens</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Tower</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Tree</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$J$51:$J$58</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>0.89400000000000002</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.2190000000000001</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.284</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.67</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.627</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.82299999999999995</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.89800000000000002</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.72399999999999998</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000007-AE3A-4D9F-95A0-33FB5FBC7371}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="1779942351"/>
+        <c:axId val="1779954415"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="1779942351"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="LID4096"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1779954415"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1779954415"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="LID4096"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1779942351"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="LID4096"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="LID4096"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>DC</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> Miss Rate</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="LID4096"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$C$62</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>64</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$B$63:$B$70</c:f>
+              <c:strCache>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>Sort</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Bubble</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Matrix</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Perm</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Puzzle</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Queens</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Tower</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Tree</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$C$63:$C$70</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>42.52</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>33.369999999999997</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>53.76</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>38.479999999999997</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>82.2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>65.94</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>54.47</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>80.17</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-9701-4C01-A27D-9D75CF329F64}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$D$62</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>128</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$B$63:$B$70</c:f>
+              <c:strCache>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>Sort</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Bubble</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Matrix</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Perm</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Puzzle</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Queens</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Tower</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Tree</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$D$63:$D$70</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>36.880000000000003</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>32.130000000000003</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>44.88</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>25.11</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>80.62</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>57.63</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>49.86</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>75.41</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-9701-4C01-A27D-9D75CF329F64}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$E$62</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>256</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent3"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$B$63:$B$70</c:f>
+              <c:strCache>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>Sort</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Bubble</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Matrix</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Perm</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Puzzle</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Queens</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Tower</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Tree</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$E$63:$E$70</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>26.88</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>27.18</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>38</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>7.64</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>74.290000000000006</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>41.59</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>36.17</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>65.739999999999995</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-9701-4C01-A27D-9D75CF329F64}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$F$62</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>512</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent4"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$B$63:$B$70</c:f>
+              <c:strCache>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>Sort</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Bubble</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Matrix</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Perm</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Puzzle</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Queens</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Tower</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Tree</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$F$63:$F$70</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>19.05</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>9.5399999999999991</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>31.42</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.37</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>66.540000000000006</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>20.7</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>14.14</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>52.24</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-9701-4C01-A27D-9D75CF329F64}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$G$62</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>1024</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent5"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$B$63:$B$70</c:f>
+              <c:strCache>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>Sort</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Bubble</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Matrix</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Perm</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Puzzle</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Queens</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Tower</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Tree</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$G$63:$G$70</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>12.1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.36</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>28.84</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.04</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>60.21</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>14.75</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7.93</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>34.54</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000004-9701-4C01-A27D-9D75CF329F64}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$H$62</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>2048</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent6"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$B$63:$B$70</c:f>
+              <c:strCache>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>Sort</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Bubble</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Matrix</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Perm</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Puzzle</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Queens</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Tower</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Tree</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$H$63:$H$70</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>4.87</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.34</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>16.27</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.03</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>53.7</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.22</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7.55</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>20.69</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000005-9701-4C01-A27D-9D75CF329F64}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="6"/>
+          <c:order val="6"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$I$62</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>4096</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1">
+                <a:lumMod val="60000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$B$63:$B$70</c:f>
+              <c:strCache>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>Sort</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Bubble</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Matrix</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Perm</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Puzzle</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Queens</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Tower</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Tree</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$I$63:$I$70</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>3.76</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.34</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5.32</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.03</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>44.72</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.22</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.11</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>13.54</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000006-9701-4C01-A27D-9D75CF329F64}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="7"/>
+          <c:order val="7"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$J$62</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>8192</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2">
+                <a:lumMod val="60000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$B$63:$B$70</c:f>
+              <c:strCache>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>Sort</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Bubble</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Matrix</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Perm</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Puzzle</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Queens</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Tower</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Tree</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$J$63:$J$70</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>3.36</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.34</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.83</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.03</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>33.159999999999997</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.22</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.11</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>6.44</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000007-9701-4C01-A27D-9D75CF329F64}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="1771416111"/>
+        <c:axId val="1771424431"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="1771416111"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="LID4096"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1771424431"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1771424431"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="LID4096"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1771416111"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="LID4096"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="LID4096"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -2717,6 +4807,86 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
@@ -3221,6 +5391,1012 @@
 </file>
 
 <file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -3792,6 +6968,78 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>260106</xdr:colOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>42496</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>575164</xdr:colOff>
+      <xdr:row>59</xdr:row>
+      <xdr:rowOff>89388</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3EDFD4D3-892D-47C3-B062-01E1DA31B87C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>282087</xdr:colOff>
+      <xdr:row>59</xdr:row>
+      <xdr:rowOff>167054</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>597145</xdr:colOff>
+      <xdr:row>74</xdr:row>
+      <xdr:rowOff>23446</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="Chart 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4158C2E6-7F65-41A5-A39D-4594A9264AB4}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -4099,8 +7347,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{12438538-68C4-4DD8-AAC5-F414AD8AE85B}">
   <dimension ref="A1:V70"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="M66" sqref="M66"/>
+    <sheetView tabSelected="1" topLeftCell="A43" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="U60" sqref="U60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4261,16 +7509,16 @@
       <c r="B7" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C7" s="3" t="s">
+      <c r="C7" s="28" t="s">
         <v>9</v>
       </c>
-      <c r="D7" s="4"/>
-      <c r="E7" s="4"/>
-      <c r="F7" s="4"/>
-      <c r="G7" s="4"/>
-      <c r="H7" s="4"/>
-      <c r="I7" s="4"/>
-      <c r="J7" s="5"/>
+      <c r="D7" s="29"/>
+      <c r="E7" s="29"/>
+      <c r="F7" s="29"/>
+      <c r="G7" s="29"/>
+      <c r="H7" s="29"/>
+      <c r="I7" s="29"/>
+      <c r="J7" s="30"/>
       <c r="K7" s="1"/>
       <c r="L7" s="1"/>
       <c r="M7" s="1"/>
@@ -4287,28 +7535,28 @@
     <row r="8" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="1"/>
       <c r="B8" s="2"/>
-      <c r="C8" s="6">
+      <c r="C8" s="3">
         <v>64</v>
       </c>
-      <c r="D8" s="7">
+      <c r="D8" s="4">
         <v>128</v>
       </c>
-      <c r="E8" s="7">
+      <c r="E8" s="4">
         <v>256</v>
       </c>
-      <c r="F8" s="7">
+      <c r="F8" s="4">
         <v>512</v>
       </c>
-      <c r="G8" s="7">
+      <c r="G8" s="4">
         <v>1024</v>
       </c>
-      <c r="H8" s="7">
+      <c r="H8" s="4">
         <v>2048</v>
       </c>
-      <c r="I8" s="7">
+      <c r="I8" s="4">
         <v>4096</v>
       </c>
-      <c r="J8" s="8">
+      <c r="J8" s="5">
         <v>8192</v>
       </c>
       <c r="K8" s="1"/>
@@ -4326,31 +7574,31 @@
     </row>
     <row r="9" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
-      <c r="B9" s="9" t="s">
+      <c r="B9" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="C9" s="10">
+      <c r="C9" s="7">
         <v>0.73699999999999999</v>
       </c>
-      <c r="D9" s="11">
+      <c r="D9" s="8">
         <v>0.77300000000000002</v>
       </c>
-      <c r="E9" s="11">
+      <c r="E9" s="8">
         <v>0.77300000000000002</v>
       </c>
-      <c r="F9" s="11">
+      <c r="F9" s="8">
         <v>0.77300000000000002</v>
       </c>
-      <c r="G9" s="11">
+      <c r="G9" s="8">
         <v>0.77300000000000002</v>
       </c>
-      <c r="H9" s="11">
+      <c r="H9" s="8">
         <v>0.77300000000000002</v>
       </c>
-      <c r="I9" s="11">
+      <c r="I9" s="8">
         <v>0.77300000000000002</v>
       </c>
-      <c r="J9" s="12">
+      <c r="J9" s="9">
         <v>0.77300000000000002</v>
       </c>
       <c r="K9" s="1"/>
@@ -4368,31 +7616,31 @@
     </row>
     <row r="10" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
-      <c r="B10" s="13" t="s">
+      <c r="B10" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="C10" s="10">
+      <c r="C10" s="7">
         <v>1.1279999999999999</v>
       </c>
-      <c r="D10" s="14">
+      <c r="D10" s="11">
         <v>1.2190000000000001</v>
       </c>
-      <c r="E10" s="14">
+      <c r="E10" s="11">
         <v>1.2190000000000001</v>
       </c>
-      <c r="F10" s="14">
+      <c r="F10" s="11">
         <v>1.2190000000000001</v>
       </c>
-      <c r="G10" s="14">
+      <c r="G10" s="11">
         <v>1.2190000000000001</v>
       </c>
-      <c r="H10" s="14">
+      <c r="H10" s="11">
         <v>1.2190000000000001</v>
       </c>
-      <c r="I10" s="14">
+      <c r="I10" s="11">
         <v>1.2190000000000001</v>
       </c>
-      <c r="J10" s="15">
+      <c r="J10" s="12">
         <v>1.2190000000000001</v>
       </c>
       <c r="K10" s="1"/>
@@ -4410,31 +7658,31 @@
     </row>
     <row r="11" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
-      <c r="B11" s="13" t="s">
+      <c r="B11" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="C11" s="10">
+      <c r="C11" s="7">
         <v>0.65400000000000003</v>
       </c>
-      <c r="D11" s="14">
+      <c r="D11" s="11">
         <v>0.65400000000000003</v>
       </c>
-      <c r="E11" s="14">
+      <c r="E11" s="11">
         <v>0.65400000000000003</v>
       </c>
-      <c r="F11" s="14">
+      <c r="F11" s="11">
         <v>0.65400000000000003</v>
       </c>
-      <c r="G11" s="14">
+      <c r="G11" s="11">
         <v>0.65400000000000003</v>
       </c>
-      <c r="H11" s="14">
+      <c r="H11" s="11">
         <v>0.65400000000000003</v>
       </c>
-      <c r="I11" s="14">
+      <c r="I11" s="11">
         <v>0.65400000000000003</v>
       </c>
-      <c r="J11" s="15">
+      <c r="J11" s="12">
         <v>0.65400000000000003</v>
       </c>
       <c r="K11" s="1"/>
@@ -4452,31 +7700,31 @@
     </row>
     <row r="12" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
-      <c r="B12" s="13" t="s">
+      <c r="B12" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="C12" s="10">
+      <c r="C12" s="7">
         <v>0.505</v>
       </c>
-      <c r="D12" s="14">
+      <c r="D12" s="11">
         <v>0.67</v>
       </c>
-      <c r="E12" s="14">
+      <c r="E12" s="11">
         <v>0.67</v>
       </c>
-      <c r="F12" s="14">
+      <c r="F12" s="11">
         <v>0.67</v>
       </c>
-      <c r="G12" s="14">
+      <c r="G12" s="11">
         <v>0.67</v>
       </c>
-      <c r="H12" s="14">
+      <c r="H12" s="11">
         <v>0.67</v>
       </c>
-      <c r="I12" s="14">
+      <c r="I12" s="11">
         <v>0.67</v>
       </c>
-      <c r="J12" s="15">
+      <c r="J12" s="12">
         <v>0.67</v>
       </c>
       <c r="K12" s="1"/>
@@ -4494,31 +7742,31 @@
     </row>
     <row r="13" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
-      <c r="B13" s="13" t="s">
+      <c r="B13" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="C13" s="10">
+      <c r="C13" s="7">
         <v>0.45500000000000002</v>
       </c>
-      <c r="D13" s="14">
+      <c r="D13" s="11">
         <v>0.46</v>
       </c>
-      <c r="E13" s="14">
+      <c r="E13" s="11">
         <v>0.49199999999999999</v>
       </c>
-      <c r="F13" s="14">
+      <c r="F13" s="11">
         <v>0.49199999999999999</v>
       </c>
-      <c r="G13" s="14">
+      <c r="G13" s="11">
         <v>0.49199999999999999</v>
       </c>
-      <c r="H13" s="14">
+      <c r="H13" s="11">
         <v>0.49199999999999999</v>
       </c>
-      <c r="I13" s="14">
+      <c r="I13" s="11">
         <v>0.49199999999999999</v>
       </c>
-      <c r="J13" s="15">
+      <c r="J13" s="12">
         <v>0.49199999999999999</v>
       </c>
       <c r="K13" s="1"/>
@@ -4536,31 +7784,31 @@
     </row>
     <row r="14" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
-      <c r="B14" s="13" t="s">
+      <c r="B14" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="C14" s="10">
+      <c r="C14" s="7">
         <v>0.60799999999999998</v>
       </c>
-      <c r="D14" s="14">
+      <c r="D14" s="11">
         <v>0.69099999999999995</v>
       </c>
-      <c r="E14" s="14">
+      <c r="E14" s="11">
         <v>0.69199999999999995</v>
       </c>
-      <c r="F14" s="14">
+      <c r="F14" s="11">
         <v>0.69199999999999995</v>
       </c>
-      <c r="G14" s="14">
+      <c r="G14" s="11">
         <v>0.69199999999999995</v>
       </c>
-      <c r="H14" s="14">
+      <c r="H14" s="11">
         <v>0.69199999999999995</v>
       </c>
-      <c r="I14" s="14">
+      <c r="I14" s="11">
         <v>0.69199999999999995</v>
       </c>
-      <c r="J14" s="15">
+      <c r="J14" s="12">
         <v>0.69199999999999995</v>
       </c>
       <c r="K14" s="1"/>
@@ -4578,31 +7826,31 @@
     </row>
     <row r="15" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
-      <c r="B15" s="13" t="s">
+      <c r="B15" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="C15" s="10">
+      <c r="C15" s="7">
         <v>0.45</v>
       </c>
-      <c r="D15" s="14">
+      <c r="D15" s="11">
         <v>0.56399999999999995</v>
       </c>
-      <c r="E15" s="14">
+      <c r="E15" s="11">
         <v>0.73199999999999998</v>
       </c>
-      <c r="F15" s="14">
+      <c r="F15" s="11">
         <v>0.73199999999999998</v>
       </c>
-      <c r="G15" s="14">
+      <c r="G15" s="11">
         <v>0.73199999999999998</v>
       </c>
-      <c r="H15" s="14">
+      <c r="H15" s="11">
         <v>0.73199999999999998</v>
       </c>
-      <c r="I15" s="14">
+      <c r="I15" s="11">
         <v>0.73199999999999998</v>
       </c>
-      <c r="J15" s="15">
+      <c r="J15" s="12">
         <v>0.73199999999999998</v>
       </c>
       <c r="K15" s="1"/>
@@ -4620,31 +7868,31 @@
     </row>
     <row r="16" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="1"/>
-      <c r="B16" s="16" t="s">
+      <c r="B16" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="C16" s="17">
+      <c r="C16" s="14">
         <v>0.46200000000000002</v>
       </c>
-      <c r="D16" s="18">
+      <c r="D16" s="15">
         <v>0.47799999999999998</v>
       </c>
-      <c r="E16" s="18">
+      <c r="E16" s="15">
         <v>0.51400000000000001</v>
       </c>
-      <c r="F16" s="18">
+      <c r="F16" s="15">
         <v>0.51400000000000001</v>
       </c>
-      <c r="G16" s="18">
+      <c r="G16" s="15">
         <v>0.51400000000000001</v>
       </c>
-      <c r="H16" s="18">
+      <c r="H16" s="15">
         <v>0.51400000000000001</v>
       </c>
-      <c r="I16" s="18">
+      <c r="I16" s="15">
         <v>0.51400000000000001</v>
       </c>
-      <c r="J16" s="19">
+      <c r="J16" s="16">
         <v>0.51400000000000001</v>
       </c>
       <c r="K16" s="1"/>
@@ -4833,16 +8081,16 @@
       <c r="B24" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C24" s="3" t="s">
+      <c r="C24" s="28" t="s">
         <v>9</v>
       </c>
-      <c r="D24" s="4"/>
-      <c r="E24" s="4"/>
-      <c r="F24" s="4"/>
-      <c r="G24" s="4"/>
-      <c r="H24" s="4"/>
-      <c r="I24" s="4"/>
-      <c r="J24" s="5"/>
+      <c r="D24" s="29"/>
+      <c r="E24" s="29"/>
+      <c r="F24" s="29"/>
+      <c r="G24" s="29"/>
+      <c r="H24" s="29"/>
+      <c r="I24" s="29"/>
+      <c r="J24" s="30"/>
       <c r="K24" s="1"/>
       <c r="L24" s="1"/>
       <c r="M24" s="1"/>
@@ -4859,28 +8107,28 @@
     <row r="25" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="1"/>
       <c r="B25" s="2"/>
-      <c r="C25" s="6">
+      <c r="C25" s="3">
         <v>64</v>
       </c>
-      <c r="D25" s="7">
+      <c r="D25" s="4">
         <v>128</v>
       </c>
-      <c r="E25" s="7">
+      <c r="E25" s="4">
         <v>256</v>
       </c>
-      <c r="F25" s="7">
+      <c r="F25" s="4">
         <v>512</v>
       </c>
-      <c r="G25" s="7">
+      <c r="G25" s="4">
         <v>1024</v>
       </c>
-      <c r="H25" s="7">
+      <c r="H25" s="4">
         <v>2048</v>
       </c>
-      <c r="I25" s="7">
+      <c r="I25" s="4">
         <v>4096</v>
       </c>
-      <c r="J25" s="8">
+      <c r="J25" s="5">
         <v>8192</v>
       </c>
       <c r="K25" s="1"/>
@@ -4898,31 +8146,31 @@
     </row>
     <row r="26" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A26" s="1"/>
-      <c r="B26" s="9" t="s">
+      <c r="B26" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="C26" s="10">
+      <c r="C26" s="7">
         <v>4.7</v>
       </c>
-      <c r="D26" s="11">
+      <c r="D26" s="8">
         <v>0.12</v>
       </c>
-      <c r="E26" s="11">
+      <c r="E26" s="8">
         <v>0.11</v>
       </c>
-      <c r="F26" s="11">
+      <c r="F26" s="8">
         <v>0.11</v>
       </c>
-      <c r="G26" s="11">
+      <c r="G26" s="8">
         <v>0.11</v>
       </c>
-      <c r="H26" s="11">
+      <c r="H26" s="8">
         <v>0.11</v>
       </c>
-      <c r="I26" s="11">
+      <c r="I26" s="8">
         <v>0.11</v>
       </c>
-      <c r="J26" s="12">
+      <c r="J26" s="9">
         <v>0.11</v>
       </c>
       <c r="K26" s="1"/>
@@ -4940,31 +8188,31 @@
     </row>
     <row r="27" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A27" s="1"/>
-      <c r="B27" s="13" t="s">
+      <c r="B27" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="C27" s="20">
+      <c r="C27" s="17">
         <v>0.05</v>
       </c>
-      <c r="D27" s="14">
+      <c r="D27" s="11">
         <v>0.04</v>
       </c>
-      <c r="E27" s="14">
+      <c r="E27" s="11">
         <v>0.04</v>
       </c>
-      <c r="F27" s="14">
+      <c r="F27" s="11">
         <v>0.04</v>
       </c>
-      <c r="G27" s="14">
+      <c r="G27" s="11">
         <v>0.04</v>
       </c>
-      <c r="H27" s="14">
+      <c r="H27" s="11">
         <v>0.04</v>
       </c>
-      <c r="I27" s="14">
+      <c r="I27" s="11">
         <v>0.04</v>
       </c>
-      <c r="J27" s="15">
+      <c r="J27" s="12">
         <v>0.04</v>
       </c>
       <c r="K27" s="1"/>
@@ -4982,31 +8230,31 @@
     </row>
     <row r="28" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A28" s="1"/>
-      <c r="B28" s="13" t="s">
+      <c r="B28" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="C28" s="20">
+      <c r="C28" s="17">
         <v>0.06</v>
       </c>
-      <c r="D28" s="14">
+      <c r="D28" s="11">
         <v>0.05</v>
       </c>
-      <c r="E28" s="14">
+      <c r="E28" s="11">
         <v>0.04</v>
       </c>
-      <c r="F28" s="14">
+      <c r="F28" s="11">
         <v>0.04</v>
       </c>
-      <c r="G28" s="14">
+      <c r="G28" s="11">
         <v>0.04</v>
       </c>
-      <c r="H28" s="14">
+      <c r="H28" s="11">
         <v>0.04</v>
       </c>
-      <c r="I28" s="14">
+      <c r="I28" s="11">
         <v>0.04</v>
       </c>
-      <c r="J28" s="15">
+      <c r="J28" s="12">
         <v>0.04</v>
       </c>
       <c r="K28" s="1"/>
@@ -5024,31 +8272,31 @@
     </row>
     <row r="29" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A29" s="1"/>
-      <c r="B29" s="13" t="s">
+      <c r="B29" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="C29" s="20">
+      <c r="C29" s="17">
         <v>26.13</v>
       </c>
-      <c r="D29" s="14">
+      <c r="D29" s="11">
         <v>0.01</v>
       </c>
-      <c r="E29" s="14">
+      <c r="E29" s="11">
         <v>0.01</v>
       </c>
-      <c r="F29" s="14">
+      <c r="F29" s="11">
         <v>0.01</v>
       </c>
-      <c r="G29" s="14">
+      <c r="G29" s="11">
         <v>0.01</v>
       </c>
-      <c r="H29" s="14">
+      <c r="H29" s="11">
         <v>0.01</v>
       </c>
-      <c r="I29" s="14">
+      <c r="I29" s="11">
         <v>0.01</v>
       </c>
-      <c r="J29" s="15">
+      <c r="J29" s="12">
         <v>0.01</v>
       </c>
       <c r="K29" s="1"/>
@@ -5066,31 +8314,31 @@
     </row>
     <row r="30" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A30" s="1"/>
-      <c r="B30" s="13" t="s">
+      <c r="B30" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="C30" s="20">
+      <c r="C30" s="17">
         <v>12</v>
       </c>
-      <c r="D30" s="14">
+      <c r="D30" s="11">
         <v>10.24</v>
       </c>
-      <c r="E30" s="14">
+      <c r="E30" s="11">
         <v>0.04</v>
       </c>
-      <c r="F30" s="14">
+      <c r="F30" s="11">
         <v>0.04</v>
       </c>
-      <c r="G30" s="14">
+      <c r="G30" s="11">
         <v>0.04</v>
       </c>
-      <c r="H30" s="14">
+      <c r="H30" s="11">
         <v>0.04</v>
       </c>
-      <c r="I30" s="14">
+      <c r="I30" s="11">
         <v>0.04</v>
       </c>
-      <c r="J30" s="15">
+      <c r="J30" s="12">
         <v>0.04</v>
       </c>
       <c r="K30" s="1"/>
@@ -5108,31 +8356,31 @@
     </row>
     <row r="31" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A31" s="1"/>
-      <c r="B31" s="13" t="s">
+      <c r="B31" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="C31" s="20">
+      <c r="C31" s="17">
         <v>13.2</v>
       </c>
-      <c r="D31" s="14">
+      <c r="D31" s="11">
         <v>0.16</v>
       </c>
-      <c r="E31" s="14">
+      <c r="E31" s="11">
         <v>0.04</v>
       </c>
-      <c r="F31" s="14">
+      <c r="F31" s="11">
         <v>0.04</v>
       </c>
-      <c r="G31" s="14">
+      <c r="G31" s="11">
         <v>0.04</v>
       </c>
-      <c r="H31" s="14">
+      <c r="H31" s="11">
         <v>0.04</v>
       </c>
-      <c r="I31" s="14">
+      <c r="I31" s="11">
         <v>0.04</v>
       </c>
-      <c r="J31" s="15">
+      <c r="J31" s="12">
         <v>0.04</v>
       </c>
       <c r="K31" s="1"/>
@@ -5150,31 +8398,31 @@
     </row>
     <row r="32" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A32" s="1"/>
-      <c r="B32" s="13" t="s">
+      <c r="B32" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="C32" s="20">
+      <c r="C32" s="17">
         <v>61.7</v>
       </c>
-      <c r="D32" s="14">
+      <c r="D32" s="11">
         <v>29.35</v>
       </c>
-      <c r="E32" s="14">
+      <c r="E32" s="11">
         <v>0.05</v>
       </c>
-      <c r="F32" s="14">
+      <c r="F32" s="11">
         <v>0.05</v>
       </c>
-      <c r="G32" s="14">
+      <c r="G32" s="11">
         <v>0.05</v>
       </c>
-      <c r="H32" s="14">
+      <c r="H32" s="11">
         <v>0.05</v>
       </c>
-      <c r="I32" s="14">
+      <c r="I32" s="11">
         <v>0.05</v>
       </c>
-      <c r="J32" s="15">
+      <c r="J32" s="12">
         <v>0.05</v>
       </c>
       <c r="K32" s="1"/>
@@ -5192,31 +8440,31 @@
     </row>
     <row r="33" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="1"/>
-      <c r="B33" s="16" t="s">
+      <c r="B33" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="C33" s="21">
+      <c r="C33" s="18">
         <v>12.94</v>
       </c>
-      <c r="D33" s="18">
+      <c r="D33" s="15">
         <v>8.65</v>
       </c>
-      <c r="E33" s="18">
+      <c r="E33" s="15">
         <v>0.06</v>
       </c>
-      <c r="F33" s="18">
+      <c r="F33" s="15">
         <v>0.06</v>
       </c>
-      <c r="G33" s="18">
+      <c r="G33" s="15">
         <v>0.06</v>
       </c>
-      <c r="H33" s="18">
+      <c r="H33" s="15">
         <v>0.06</v>
       </c>
-      <c r="I33" s="18">
+      <c r="I33" s="15">
         <v>0.06</v>
       </c>
-      <c r="J33" s="19">
+      <c r="J33" s="16">
         <v>0.06</v>
       </c>
       <c r="K33" s="1"/>
@@ -5512,294 +8760,550 @@
       <c r="B49" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C49" s="3" t="s">
+      <c r="C49" s="28" t="s">
         <v>14</v>
       </c>
-      <c r="D49" s="4"/>
-      <c r="E49" s="4"/>
-      <c r="F49" s="4"/>
-      <c r="G49" s="4"/>
-      <c r="H49" s="4"/>
-      <c r="I49" s="4"/>
-      <c r="J49" s="5"/>
+      <c r="D49" s="29"/>
+      <c r="E49" s="29"/>
+      <c r="F49" s="29"/>
+      <c r="G49" s="29"/>
+      <c r="H49" s="29"/>
+      <c r="I49" s="29"/>
+      <c r="J49" s="30"/>
     </row>
     <row r="50" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B50" s="2"/>
-      <c r="C50" s="25">
+      <c r="C50" s="22">
         <v>64</v>
       </c>
-      <c r="D50" s="26">
+      <c r="D50" s="23">
         <v>128</v>
       </c>
-      <c r="E50" s="26">
+      <c r="E50" s="23">
         <v>256</v>
       </c>
-      <c r="F50" s="26">
+      <c r="F50" s="23">
         <v>512</v>
       </c>
-      <c r="G50" s="26">
+      <c r="G50" s="23">
         <v>1024</v>
       </c>
-      <c r="H50" s="26">
+      <c r="H50" s="23">
         <v>2048</v>
       </c>
-      <c r="I50" s="26">
+      <c r="I50" s="23">
         <v>4096</v>
       </c>
-      <c r="J50" s="27">
+      <c r="J50" s="24">
         <v>8192</v>
       </c>
     </row>
     <row r="51" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B51" s="22" t="s">
+      <c r="B51" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="C51" s="28"/>
-      <c r="D51" s="29"/>
-      <c r="E51" s="29"/>
-      <c r="F51" s="29"/>
-      <c r="G51" s="29"/>
-      <c r="H51" s="29"/>
-      <c r="I51" s="29"/>
-      <c r="J51" s="30"/>
+      <c r="C51" s="25">
+        <v>0.52900000000000003</v>
+      </c>
+      <c r="D51" s="26">
+        <v>0.56699999999999995</v>
+      </c>
+      <c r="E51" s="26">
+        <v>0.63800000000000001</v>
+      </c>
+      <c r="F51" s="26">
+        <v>0.70099999999999996</v>
+      </c>
+      <c r="G51" s="26">
+        <v>0.77300000000000002</v>
+      </c>
+      <c r="H51" s="26">
+        <v>0.875</v>
+      </c>
+      <c r="I51" s="26">
+        <v>0.88900000000000001</v>
+      </c>
+      <c r="J51" s="27">
+        <v>0.89400000000000002</v>
+      </c>
     </row>
     <row r="52" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B52" s="23" t="s">
+      <c r="B52" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="C52" s="20"/>
-      <c r="D52" s="14"/>
-      <c r="E52" s="14"/>
-      <c r="F52" s="14"/>
-      <c r="G52" s="14"/>
-      <c r="H52" s="14"/>
-      <c r="I52" s="14"/>
-      <c r="J52" s="15"/>
+      <c r="C52" s="17">
+        <v>0.55700000000000005</v>
+      </c>
+      <c r="D52" s="11">
+        <v>0.56799999999999995</v>
+      </c>
+      <c r="E52" s="11">
+        <v>0.62</v>
+      </c>
+      <c r="F52" s="11">
+        <v>0.91600000000000004</v>
+      </c>
+      <c r="G52" s="11">
+        <v>1.2190000000000001</v>
+      </c>
+      <c r="H52" s="11">
+        <v>1.2190000000000001</v>
+      </c>
+      <c r="I52" s="11">
+        <v>1.2190000000000001</v>
+      </c>
+      <c r="J52" s="12">
+        <v>1.2190000000000001</v>
+      </c>
     </row>
     <row r="53" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B53" s="23" t="s">
+      <c r="B53" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="C53" s="20"/>
-      <c r="D53" s="14"/>
-      <c r="E53" s="14"/>
-      <c r="F53" s="14"/>
-      <c r="G53" s="14"/>
-      <c r="H53" s="14"/>
-      <c r="I53" s="14"/>
-      <c r="J53" s="15"/>
+      <c r="C53" s="17">
+        <v>0.44500000000000001</v>
+      </c>
+      <c r="D53" s="11">
+        <v>0.502</v>
+      </c>
+      <c r="E53" s="11">
+        <v>0.55700000000000005</v>
+      </c>
+      <c r="F53" s="11">
+        <v>0.624</v>
+      </c>
+      <c r="G53" s="11">
+        <v>0.65400000000000003</v>
+      </c>
+      <c r="H53" s="11">
+        <v>0.85699999999999998</v>
+      </c>
+      <c r="I53" s="11">
+        <v>1.1759999999999999</v>
+      </c>
+      <c r="J53" s="12">
+        <v>1.284</v>
+      </c>
     </row>
     <row r="54" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B54" s="23" t="s">
+      <c r="B54" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="C54" s="20"/>
-      <c r="D54" s="14"/>
-      <c r="E54" s="14"/>
-      <c r="F54" s="14"/>
-      <c r="G54" s="14"/>
-      <c r="H54" s="14"/>
-      <c r="I54" s="14"/>
-      <c r="J54" s="15"/>
+      <c r="C54" s="17">
+        <v>0.43</v>
+      </c>
+      <c r="D54" s="11">
+        <v>0.5</v>
+      </c>
+      <c r="E54" s="11">
+        <v>0.60699999999999998</v>
+      </c>
+      <c r="F54" s="11">
+        <v>0.66700000000000004</v>
+      </c>
+      <c r="G54" s="11">
+        <v>0.67</v>
+      </c>
+      <c r="H54" s="11">
+        <v>0.67</v>
+      </c>
+      <c r="I54" s="11">
+        <v>0.67</v>
+      </c>
+      <c r="J54" s="12">
+        <v>0.67</v>
+      </c>
     </row>
     <row r="55" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B55" s="23" t="s">
+      <c r="B55" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="C55" s="20"/>
-      <c r="D55" s="14"/>
-      <c r="E55" s="14"/>
-      <c r="F55" s="14"/>
-      <c r="G55" s="14"/>
-      <c r="H55" s="14"/>
-      <c r="I55" s="14"/>
-      <c r="J55" s="15"/>
+      <c r="C55" s="17">
+        <v>0.41899999999999998</v>
+      </c>
+      <c r="D55" s="11">
+        <v>0.42299999999999999</v>
+      </c>
+      <c r="E55" s="11">
+        <v>0.443</v>
+      </c>
+      <c r="F55" s="11">
+        <v>0.46899999999999997</v>
+      </c>
+      <c r="G55" s="11">
+        <v>0.49199999999999999</v>
+      </c>
+      <c r="H55" s="11">
+        <v>0.51400000000000001</v>
+      </c>
+      <c r="I55" s="11">
+        <v>0.55800000000000005</v>
+      </c>
+      <c r="J55" s="12">
+        <v>0.627</v>
+      </c>
     </row>
     <row r="56" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B56" s="23" t="s">
+      <c r="B56" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="C56" s="20"/>
-      <c r="D56" s="14"/>
-      <c r="E56" s="14"/>
-      <c r="F56" s="14"/>
-      <c r="G56" s="14"/>
-      <c r="H56" s="14"/>
-      <c r="I56" s="14"/>
-      <c r="J56" s="15"/>
+      <c r="C56" s="17">
+        <v>0.39100000000000001</v>
+      </c>
+      <c r="D56" s="11">
+        <v>0.41899999999999998</v>
+      </c>
+      <c r="E56" s="11">
+        <v>0.48399999999999999</v>
+      </c>
+      <c r="F56" s="11">
+        <v>0.63</v>
+      </c>
+      <c r="G56" s="11">
+        <v>0.69199999999999995</v>
+      </c>
+      <c r="H56" s="11">
+        <v>0.82299999999999995</v>
+      </c>
+      <c r="I56" s="11">
+        <v>0.82299999999999995</v>
+      </c>
+      <c r="J56" s="12">
+        <v>0.82299999999999995</v>
+      </c>
     </row>
     <row r="57" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B57" s="23" t="s">
+      <c r="B57" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="C57" s="20"/>
-      <c r="D57" s="14"/>
-      <c r="E57" s="14"/>
-      <c r="F57" s="14"/>
-      <c r="G57" s="14"/>
-      <c r="H57" s="14"/>
-      <c r="I57" s="14"/>
-      <c r="J57" s="15"/>
+      <c r="C57" s="17">
+        <v>0.443</v>
+      </c>
+      <c r="D57" s="11">
+        <v>0.497</v>
+      </c>
+      <c r="E57" s="11">
+        <v>0.52400000000000002</v>
+      </c>
+      <c r="F57" s="11">
+        <v>0.67300000000000004</v>
+      </c>
+      <c r="G57" s="11">
+        <v>0.73199999999999998</v>
+      </c>
+      <c r="H57" s="11">
+        <v>0.73599999999999999</v>
+      </c>
+      <c r="I57" s="11">
+        <v>0.89800000000000002</v>
+      </c>
+      <c r="J57" s="12">
+        <v>0.89800000000000002</v>
+      </c>
     </row>
     <row r="58" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B58" s="24" t="s">
+      <c r="B58" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="C58" s="21"/>
-      <c r="D58" s="18"/>
-      <c r="E58" s="18"/>
-      <c r="F58" s="18"/>
-      <c r="G58" s="18"/>
-      <c r="H58" s="18"/>
-      <c r="I58" s="18"/>
-      <c r="J58" s="19"/>
+      <c r="C58" s="18">
+        <v>0.35799999999999998</v>
+      </c>
+      <c r="D58" s="15">
+        <v>0.373</v>
+      </c>
+      <c r="E58" s="15">
+        <v>0.40200000000000002</v>
+      </c>
+      <c r="F58" s="15">
+        <v>0.44600000000000001</v>
+      </c>
+      <c r="G58" s="15">
+        <v>0.51400000000000001</v>
+      </c>
+      <c r="H58" s="15">
+        <v>0.58599999999999997</v>
+      </c>
+      <c r="I58" s="15">
+        <v>0.625</v>
+      </c>
+      <c r="J58" s="16">
+        <v>0.72399999999999998</v>
+      </c>
     </row>
     <row r="60" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="61" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B61" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C61" s="3" t="s">
+      <c r="C61" s="28" t="s">
         <v>14</v>
       </c>
-      <c r="D61" s="4"/>
-      <c r="E61" s="4"/>
-      <c r="F61" s="4"/>
-      <c r="G61" s="4"/>
-      <c r="H61" s="4"/>
-      <c r="I61" s="4"/>
-      <c r="J61" s="5"/>
+      <c r="D61" s="29"/>
+      <c r="E61" s="29"/>
+      <c r="F61" s="29"/>
+      <c r="G61" s="29"/>
+      <c r="H61" s="29"/>
+      <c r="I61" s="29"/>
+      <c r="J61" s="30"/>
     </row>
     <row r="62" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B62" s="2"/>
-      <c r="C62" s="25">
+      <c r="C62" s="22">
         <v>64</v>
       </c>
-      <c r="D62" s="26">
+      <c r="D62" s="23">
         <v>128</v>
       </c>
-      <c r="E62" s="26">
+      <c r="E62" s="23">
         <v>256</v>
       </c>
-      <c r="F62" s="26">
+      <c r="F62" s="23">
         <v>512</v>
       </c>
-      <c r="G62" s="26">
+      <c r="G62" s="23">
         <v>1024</v>
       </c>
-      <c r="H62" s="26">
+      <c r="H62" s="23">
         <v>2048</v>
       </c>
-      <c r="I62" s="26">
+      <c r="I62" s="23">
         <v>4096</v>
       </c>
-      <c r="J62" s="27">
+      <c r="J62" s="24">
         <v>8192</v>
       </c>
     </row>
     <row r="63" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B63" s="22" t="s">
+      <c r="B63" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="C63" s="28"/>
-      <c r="D63" s="29"/>
-      <c r="E63" s="29"/>
-      <c r="F63" s="29"/>
-      <c r="G63" s="29"/>
-      <c r="H63" s="29"/>
-      <c r="I63" s="29"/>
-      <c r="J63" s="30"/>
+      <c r="C63" s="25">
+        <v>42.52</v>
+      </c>
+      <c r="D63" s="26">
+        <v>36.880000000000003</v>
+      </c>
+      <c r="E63" s="26">
+        <v>26.88</v>
+      </c>
+      <c r="F63" s="26">
+        <v>19.05</v>
+      </c>
+      <c r="G63" s="26">
+        <v>12.1</v>
+      </c>
+      <c r="H63" s="26">
+        <v>4.87</v>
+      </c>
+      <c r="I63" s="26">
+        <v>3.76</v>
+      </c>
+      <c r="J63" s="27">
+        <v>3.36</v>
+      </c>
     </row>
     <row r="64" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B64" s="23" t="s">
+      <c r="B64" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="C64" s="20"/>
-      <c r="D64" s="14"/>
-      <c r="E64" s="14"/>
-      <c r="F64" s="14"/>
-      <c r="G64" s="14"/>
-      <c r="H64" s="14"/>
-      <c r="I64" s="14"/>
-      <c r="J64" s="15"/>
+      <c r="C64" s="17">
+        <v>33.369999999999997</v>
+      </c>
+      <c r="D64" s="11">
+        <v>32.130000000000003</v>
+      </c>
+      <c r="E64" s="11">
+        <v>27.18</v>
+      </c>
+      <c r="F64" s="11">
+        <v>9.5399999999999991</v>
+      </c>
+      <c r="G64" s="11">
+        <v>0.36</v>
+      </c>
+      <c r="H64" s="11">
+        <v>0.34</v>
+      </c>
+      <c r="I64" s="11">
+        <v>0.34</v>
+      </c>
+      <c r="J64" s="12">
+        <v>0.34</v>
+      </c>
     </row>
     <row r="65" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B65" s="23" t="s">
+      <c r="B65" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="C65" s="20"/>
-      <c r="D65" s="14"/>
-      <c r="E65" s="14"/>
-      <c r="F65" s="14"/>
-      <c r="G65" s="14"/>
-      <c r="H65" s="14"/>
-      <c r="I65" s="14"/>
-      <c r="J65" s="15"/>
+      <c r="C65" s="17">
+        <v>53.76</v>
+      </c>
+      <c r="D65" s="11">
+        <v>44.88</v>
+      </c>
+      <c r="E65" s="11">
+        <v>38</v>
+      </c>
+      <c r="F65" s="11">
+        <v>31.42</v>
+      </c>
+      <c r="G65" s="11">
+        <v>28.84</v>
+      </c>
+      <c r="H65" s="11">
+        <v>16.27</v>
+      </c>
+      <c r="I65" s="11">
+        <v>5.32</v>
+      </c>
+      <c r="J65" s="12">
+        <v>2.83</v>
+      </c>
     </row>
     <row r="66" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B66" s="23" t="s">
+      <c r="B66" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="C66" s="20"/>
-      <c r="D66" s="14"/>
-      <c r="E66" s="14"/>
-      <c r="F66" s="14"/>
-      <c r="G66" s="14"/>
-      <c r="H66" s="14"/>
-      <c r="I66" s="14"/>
-      <c r="J66" s="15"/>
+      <c r="C66" s="17">
+        <v>38.479999999999997</v>
+      </c>
+      <c r="D66" s="11">
+        <v>25.11</v>
+      </c>
+      <c r="E66" s="11">
+        <v>7.64</v>
+      </c>
+      <c r="F66" s="11">
+        <v>0.37</v>
+      </c>
+      <c r="G66" s="11">
+        <v>0.04</v>
+      </c>
+      <c r="H66" s="11">
+        <v>0.03</v>
+      </c>
+      <c r="I66" s="11">
+        <v>0.03</v>
+      </c>
+      <c r="J66" s="12">
+        <v>0.03</v>
+      </c>
     </row>
     <row r="67" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B67" s="23" t="s">
+      <c r="B67" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="C67" s="20"/>
-      <c r="D67" s="14"/>
-      <c r="E67" s="14"/>
-      <c r="F67" s="14"/>
-      <c r="G67" s="14"/>
-      <c r="H67" s="14"/>
-      <c r="I67" s="14"/>
-      <c r="J67" s="15"/>
+      <c r="C67" s="17">
+        <v>82.2</v>
+      </c>
+      <c r="D67" s="11">
+        <v>80.62</v>
+      </c>
+      <c r="E67" s="11">
+        <v>74.290000000000006</v>
+      </c>
+      <c r="F67" s="11">
+        <v>66.540000000000006</v>
+      </c>
+      <c r="G67" s="11">
+        <v>60.21</v>
+      </c>
+      <c r="H67" s="11">
+        <v>53.7</v>
+      </c>
+      <c r="I67" s="11">
+        <v>44.72</v>
+      </c>
+      <c r="J67" s="12">
+        <v>33.159999999999997</v>
+      </c>
     </row>
     <row r="68" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B68" s="23" t="s">
+      <c r="B68" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="C68" s="20"/>
-      <c r="D68" s="14"/>
-      <c r="E68" s="14"/>
-      <c r="F68" s="14"/>
-      <c r="G68" s="14"/>
-      <c r="H68" s="14"/>
-      <c r="I68" s="14"/>
-      <c r="J68" s="15"/>
+      <c r="C68" s="17">
+        <v>65.94</v>
+      </c>
+      <c r="D68" s="11">
+        <v>57.63</v>
+      </c>
+      <c r="E68" s="11">
+        <v>41.59</v>
+      </c>
+      <c r="F68" s="11">
+        <v>20.7</v>
+      </c>
+      <c r="G68" s="11">
+        <v>14.75</v>
+      </c>
+      <c r="H68" s="11">
+        <v>0.22</v>
+      </c>
+      <c r="I68" s="11">
+        <v>0.22</v>
+      </c>
+      <c r="J68" s="12">
+        <v>0.22</v>
+      </c>
     </row>
     <row r="69" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B69" s="23" t="s">
+      <c r="B69" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="C69" s="20"/>
-      <c r="D69" s="14"/>
-      <c r="E69" s="14"/>
-      <c r="F69" s="14"/>
-      <c r="G69" s="14"/>
-      <c r="H69" s="14"/>
-      <c r="I69" s="14"/>
-      <c r="J69" s="15"/>
+      <c r="C69" s="17">
+        <v>54.47</v>
+      </c>
+      <c r="D69" s="11">
+        <v>49.86</v>
+      </c>
+      <c r="E69" s="11">
+        <v>36.17</v>
+      </c>
+      <c r="F69" s="11">
+        <v>14.14</v>
+      </c>
+      <c r="G69" s="11">
+        <v>7.93</v>
+      </c>
+      <c r="H69" s="11">
+        <v>7.55</v>
+      </c>
+      <c r="I69" s="11">
+        <v>0.11</v>
+      </c>
+      <c r="J69" s="12">
+        <v>0.11</v>
+      </c>
     </row>
     <row r="70" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B70" s="24" t="s">
+      <c r="B70" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="C70" s="21"/>
-      <c r="D70" s="18"/>
-      <c r="E70" s="18"/>
-      <c r="F70" s="18"/>
-      <c r="G70" s="18"/>
-      <c r="H70" s="18"/>
-      <c r="I70" s="18"/>
-      <c r="J70" s="19"/>
+      <c r="C70" s="18">
+        <v>80.17</v>
+      </c>
+      <c r="D70" s="15">
+        <v>75.41</v>
+      </c>
+      <c r="E70" s="15">
+        <v>65.739999999999995</v>
+      </c>
+      <c r="F70" s="15">
+        <v>52.24</v>
+      </c>
+      <c r="G70" s="15">
+        <v>34.54</v>
+      </c>
+      <c r="H70" s="15">
+        <v>20.69</v>
+      </c>
+      <c r="I70" s="15">
+        <v>13.54</v>
+      </c>
+      <c r="J70" s="16">
+        <v>6.44</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="4">

</xml_diff>